<commit_message>
Working draft of reading all data from ports_scenarios.  Bug in num_facility and manufacturing capacity calc
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_max.xlsx
+++ b/fabrication_ports/ports_scenario_max.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EA11C1-CD9B-4DA4-B2DB-9A91EBC4E221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAD4956-A064-4F78-AC46-0E9F58568380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$E$10:$E$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$F$10:$F$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId2"/>
+    <pivotCache cacheId="6" r:id="rId2"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="178">
   <si>
     <t>Port</t>
   </si>
@@ -395,9 +394,6 @@
     <t>Semisubmersible 3</t>
   </si>
   <si>
-    <t>Stationkeeping</t>
-  </si>
-  <si>
     <t>Mooring chain 1</t>
   </si>
   <si>
@@ -552,6 +548,30 @@
   </si>
   <si>
     <t>Floating date adder</t>
+  </si>
+  <si>
+    <t>Port upgrade cost</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Announced</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Mooring chain</t>
+  </si>
+  <si>
+    <t>Mooring rope</t>
+  </si>
+  <si>
+    <t>Production capacity</t>
+  </si>
+  <si>
+    <t>Facility cost</t>
   </si>
 </sst>
 </file>
@@ -882,7 +902,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$G$11:$G$47</c:f>
+              <c:f>'Avg Demand Scenario'!$H$11:$H$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -1140,7 +1160,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$L$11:$L$47</c:f>
+              <c:f>'Avg Demand Scenario'!$M$11:$M$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -1586,7 +1606,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$I$52</c:f>
+              <c:f>'Avg Demand Scenario'!$J$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1607,7 +1627,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$H$53:$H$71</c:f>
+              <c:f>'Avg Demand Scenario'!$I$53:$I$71</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -1669,7 +1689,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$I$53:$I$71</c:f>
+              <c:f>'Avg Demand Scenario'!$J$53:$J$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -3053,7 +3073,7 @@
       <xdr:rowOff>58177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>244928</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
@@ -3083,13 +3103,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>898921</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>75008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>2458640</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>151208</xdr:rowOff>
@@ -3123,7 +3143,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44771.490716435183" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A10:L47" sheet="Avg Demand Scenario"/>
+    <worksheetSource ref="A10:M47" sheet="Avg Demand Scenario"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Component" numFmtId="0">
@@ -3742,8 +3762,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="H52:I71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="I52:J71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -4156,109 +4176,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10:P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="82.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="8.26953125" customWidth="1"/>
+    <col min="17" max="17" width="82.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>94</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2024</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5">
+        <v>169</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>99</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D7">
+        <v>167</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -4266,40 +4291,52 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -4307,210 +4344,282 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>5</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>2021</v>
       </c>
-      <c r="H11">
-        <f>$D$6</f>
+      <c r="I11">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>5</v>
       </c>
-      <c r="J11">
-        <f>$D$3</f>
+      <c r="K11">
+        <f>$E$3</f>
         <v>0.25</v>
       </c>
-      <c r="K11">
-        <f>ROUNDDOWN(G11+H11+I11*(1-J11),0)</f>
+      <c r="L11">
+        <f>ROUNDDOWN(H11+I11+J11*(1-K11),0)</f>
         <v>2028</v>
       </c>
-      <c r="L11">
-        <f>K11-G11</f>
+      <c r="M11">
+        <f>L11-H11</f>
         <v>7</v>
       </c>
+      <c r="N11">
+        <v>150</v>
+      </c>
+      <c r="O11">
+        <v>100</v>
+      </c>
+      <c r="P11">
+        <v>300</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>5</v>
       </c>
-      <c r="G12">
-        <f>$D$4</f>
+      <c r="H12">
+        <f>$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H12">
-        <f>$D$6</f>
+      <c r="I12">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>5</v>
       </c>
-      <c r="J12">
-        <f t="shared" ref="J12:J15" si="0">$D$3</f>
+      <c r="K12">
+        <f t="shared" ref="K12:K15" si="0">$E$3</f>
         <v>0.25</v>
       </c>
-      <c r="K12">
-        <f>ROUNDDOWN(G12+H12+I12*(1-J12),0)</f>
+      <c r="L12">
+        <f>ROUNDDOWN(H12+I12+J12*(1-K12),0)</f>
         <v>2031</v>
       </c>
-      <c r="L12">
-        <f t="shared" ref="L12:L47" si="1">K12-G12</f>
+      <c r="M12">
+        <f t="shared" ref="M12:M47" si="1">L12-H12</f>
         <v>7</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12">
+        <v>150</v>
+      </c>
+      <c r="O12">
+        <v>100</v>
+      </c>
+      <c r="P12">
+        <v>300</v>
+      </c>
+      <c r="Q12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
       <c r="B13" t="s">
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D13" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>14</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>15</v>
       </c>
-      <c r="G13">
-        <f t="shared" ref="G13:G15" si="2">$D$4</f>
+      <c r="H13">
+        <f t="shared" ref="H13:H14" si="2">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H13">
-        <f>$D$6</f>
+      <c r="I13">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>5</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K13">
-        <f t="shared" ref="K13:K47" si="3">ROUNDDOWN(G13+H13+I13*(1-J13),0)</f>
+      <c r="L13">
+        <f t="shared" ref="L13:L47" si="3">ROUNDDOWN(H13+I13+J13*(1-K13),0)</f>
         <v>2031</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13">
+        <v>150</v>
+      </c>
+      <c r="O13">
+        <v>100</v>
+      </c>
+      <c r="P13">
+        <v>300</v>
+      </c>
+      <c r="Q13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
       <c r="B14" t="s">
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D14" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>24</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="2"/>
         <v>2024</v>
       </c>
-      <c r="H14">
-        <f>$D$6</f>
+      <c r="I14">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>5</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <f t="shared" si="3"/>
         <v>2031</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14">
+        <v>150</v>
+      </c>
+      <c r="O14">
+        <v>100</v>
+      </c>
+      <c r="P14">
+        <v>300</v>
+      </c>
+      <c r="Q14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" t="s">
         <v>125</v>
       </c>
-      <c r="F15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G15">
-        <f>$D$4+$D$5</f>
+      <c r="H15">
+        <f>$E$4+$E$5</f>
         <v>2025</v>
       </c>
-      <c r="H15">
-        <f>$D$6+$D$7</f>
+      <c r="I15">
+        <f>$E$6+$E$7</f>
         <v>5</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>5</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <f t="shared" si="3"/>
         <v>2033</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="N15">
+        <v>150</v>
+      </c>
+      <c r="O15">
+        <v>100</v>
+      </c>
+      <c r="P15">
+        <v>300</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -4518,164 +4627,221 @@
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="D16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" t="s">
         <v>47</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>26</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>24</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>2021</v>
       </c>
-      <c r="H16">
-        <f>$D$6</f>
+      <c r="I16">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>5</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <f t="shared" si="3"/>
         <v>2028</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16">
+        <v>150</v>
+      </c>
+      <c r="O16">
+        <v>100</v>
+      </c>
+      <c r="P16">
+        <v>300</v>
+      </c>
+      <c r="Q16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
       <c r="B17" t="s">
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" t="s">
         <v>47</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>26</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>24</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>2021</v>
       </c>
-      <c r="H17">
-        <f>$D$6</f>
+      <c r="I17">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>5</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <f t="shared" si="3"/>
         <v>2028</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17">
+        <v>150</v>
+      </c>
+      <c r="O17">
+        <v>100</v>
+      </c>
+      <c r="P17">
+        <v>300</v>
+      </c>
+      <c r="Q17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
       <c r="B18" t="s">
         <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D18" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>17</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>15</v>
       </c>
-      <c r="G18">
-        <f t="shared" ref="G18" si="4">$D$4</f>
+      <c r="H18">
+        <f t="shared" ref="H18" si="4">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H18">
-        <f>$D$6</f>
+      <c r="I18">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>5</v>
       </c>
-      <c r="J18">
-        <f t="shared" ref="J18" si="5">$D$3</f>
+      <c r="K18">
+        <f t="shared" ref="K18" si="5">$E$3</f>
         <v>0.25</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <f t="shared" si="3"/>
         <v>2031</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
+      <c r="N18">
+        <v>150</v>
+      </c>
+      <c r="O18">
+        <v>100</v>
+      </c>
+      <c r="P18">
+        <v>300</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" t="s">
-        <v>122</v>
+        <v>173</v>
+      </c>
+      <c r="D19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19">
+        <v>121</v>
+      </c>
+      <c r="G19" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19">
         <v>2023</v>
       </c>
-      <c r="H19">
-        <f>$D$6+$D$7</f>
+      <c r="I19">
+        <f>$E$6+$E$7</f>
         <v>5</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>5</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>0.25</v>
       </c>
-      <c r="K19">
-        <f t="shared" ref="K19" si="6">ROUNDDOWN(G19+H19+I19*(1-J19),0)</f>
+      <c r="L19">
+        <f t="shared" ref="L19" si="6">ROUNDDOWN(H19+I19+J19*(1-K19),0)</f>
         <v>2031</v>
       </c>
-      <c r="L19">
-        <f t="shared" ref="L19" si="7">K19-G19</f>
+      <c r="M19">
+        <f t="shared" ref="M19" si="7">L19-H19</f>
         <v>8</v>
       </c>
+      <c r="N19">
+        <v>150</v>
+      </c>
+      <c r="O19">
+        <v>100</v>
+      </c>
+      <c r="P19">
+        <v>300</v>
+      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -4683,169 +4849,226 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>24</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>2021</v>
       </c>
-      <c r="H20">
-        <f>$D$6</f>
+      <c r="I20">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>3</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>0.8</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <f t="shared" si="3"/>
         <v>2025</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20">
+        <v>150</v>
+      </c>
+      <c r="O20">
+        <v>100</v>
+      </c>
+      <c r="P20">
+        <v>300</v>
+      </c>
+      <c r="Q20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
       <c r="B21" t="s">
         <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>5</v>
       </c>
-      <c r="G21">
-        <f t="shared" ref="G21:G23" si="8">$D$4</f>
+      <c r="H21">
+        <f t="shared" ref="H21:H22" si="8">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H21">
-        <f>$D$6</f>
+      <c r="I21">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>3</v>
       </c>
-      <c r="J21">
-        <f t="shared" ref="J21:J23" si="9">$D$3</f>
+      <c r="K21">
+        <f t="shared" ref="K21:K23" si="9">$E$3</f>
         <v>0.25</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21">
+        <v>150</v>
+      </c>
+      <c r="O21">
+        <v>100</v>
+      </c>
+      <c r="P21">
+        <v>300</v>
+      </c>
+      <c r="Q21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
       <c r="B22" t="s">
         <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>152</v>
-      </c>
-      <c r="D22" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>19</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>15</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="8"/>
         <v>2024</v>
       </c>
-      <c r="H22">
-        <f>$D$6</f>
+      <c r="I22">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>3</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22">
+        <v>150</v>
+      </c>
+      <c r="O22">
+        <v>100</v>
+      </c>
+      <c r="P22">
+        <v>300</v>
+      </c>
+      <c r="Q22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" t="s">
-        <v>122</v>
+        <v>173</v>
+      </c>
+      <c r="D23" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="F23" t="s">
-        <v>126</v>
-      </c>
-      <c r="G23">
-        <f>$D$4+$D$5</f>
+        <v>121</v>
+      </c>
+      <c r="G23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23">
+        <f>$E$4+$E$5</f>
         <v>2025</v>
       </c>
-      <c r="H23">
-        <f>$D$6+$D$7</f>
+      <c r="I23">
+        <f>$E$6+$E$7</f>
         <v>5</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>3</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
-      <c r="K23">
-        <f t="shared" ref="K23" si="10">ROUNDDOWN(G23+H23+I23*(1-J23),0)</f>
+      <c r="L23">
+        <f t="shared" ref="L23" si="10">ROUNDDOWN(H23+I23+J23*(1-K23),0)</f>
         <v>2032</v>
       </c>
-      <c r="L23">
-        <f t="shared" ref="L23" si="11">K23-G23</f>
+      <c r="M23">
+        <f t="shared" ref="M23" si="11">L23-H23</f>
         <v>7</v>
       </c>
+      <c r="N23">
+        <v>150</v>
+      </c>
+      <c r="O23">
+        <v>100</v>
+      </c>
+      <c r="P23">
+        <v>300</v>
+      </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -4853,85 +5076,112 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>26</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>24</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>2020</v>
       </c>
-      <c r="H24">
-        <f>$D$6</f>
+      <c r="I24">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>2</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>0.5</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <f t="shared" si="3"/>
         <v>2025</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24">
+        <v>150</v>
+      </c>
+      <c r="O24">
+        <v>100</v>
+      </c>
+      <c r="P24">
+        <v>300</v>
+      </c>
+      <c r="Q24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
       <c r="B25" t="s">
         <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>6</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>5</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>2021</v>
       </c>
-      <c r="H25">
-        <f>$D$6</f>
+      <c r="I25">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>3.5</v>
       </c>
-      <c r="J25">
-        <f t="shared" ref="J25:J26" si="12">$D$3</f>
+      <c r="K25">
+        <f t="shared" ref="K25:K26" si="12">$E$3</f>
         <v>0.25</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <f t="shared" si="3"/>
         <v>2027</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25">
+        <v>150</v>
+      </c>
+      <c r="O25">
+        <v>100</v>
+      </c>
+      <c r="P25">
+        <v>300</v>
+      </c>
+      <c r="Q25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -4939,45 +5189,57 @@
         <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
-      </c>
-      <c r="D26" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>22</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>67</v>
       </c>
-      <c r="G26">
-        <f t="shared" ref="G26" si="13">$D$4</f>
+      <c r="H26">
+        <f t="shared" ref="H26" si="13">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H26">
-        <f>$D$6</f>
+      <c r="I26">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>2</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
-      <c r="K26">
-        <f>ROUNDDOWN(G26+H26+I26*(1-J26),0)</f>
+      <c r="L26">
+        <f>ROUNDDOWN(H26+I26+J26*(1-K26),0)</f>
         <v>2029</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26">
+        <v>150</v>
+      </c>
+      <c r="O26">
+        <v>100</v>
+      </c>
+      <c r="P26">
+        <v>300</v>
+      </c>
+      <c r="Q26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -4985,42 +5247,54 @@
         <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
-      </c>
-      <c r="D27" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>10</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>5</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>2025</v>
-      </c>
-      <c r="H27">
-        <v>2</v>
       </c>
       <c r="I27">
         <v>2</v>
       </c>
       <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
         <v>0</v>
       </c>
-      <c r="K27">
-        <f>ROUNDDOWN(G27+H27+I27*(1-J27),0)</f>
+      <c r="L27">
+        <f>ROUNDDOWN(H27+I27+J27*(1-K27),0)</f>
         <v>2029</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27">
+        <v>150</v>
+      </c>
+      <c r="O27">
+        <v>100</v>
+      </c>
+      <c r="P27">
+        <v>300</v>
+      </c>
+      <c r="Q27" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -5028,86 +5302,113 @@
         <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>23</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>24</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>2021</v>
       </c>
-      <c r="H28">
-        <f t="shared" ref="H28:H37" si="14">$D$6</f>
+      <c r="I28">
+        <f t="shared" ref="I28:I37" si="14">$E$6</f>
         <v>4</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>3</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>0.25</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <f t="shared" si="3"/>
         <v>2027</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28">
+        <v>150</v>
+      </c>
+      <c r="O28">
+        <v>100</v>
+      </c>
+      <c r="P28">
+        <v>300</v>
+      </c>
+      <c r="Q28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
       <c r="B29" t="s">
         <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>23</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>24</v>
       </c>
-      <c r="G29">
-        <f t="shared" ref="G29" si="15">$D$4</f>
+      <c r="H29">
+        <f t="shared" ref="H29" si="15">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>3</v>
       </c>
-      <c r="J29">
-        <f t="shared" ref="J29:J31" si="16">$D$3</f>
+      <c r="K29">
+        <f t="shared" ref="K29:K31" si="16">$E$3</f>
         <v>0.25</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29">
+        <v>150</v>
+      </c>
+      <c r="O29">
+        <v>100</v>
+      </c>
+      <c r="P29">
+        <v>300</v>
+      </c>
+      <c r="Q29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -5115,84 +5416,111 @@
         <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>151</v>
-      </c>
-      <c r="D30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>6</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>5</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>2021</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>6</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <f t="shared" si="16"/>
         <v>0.25</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <f t="shared" si="3"/>
         <v>2029</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="N30">
+        <v>150</v>
+      </c>
+      <c r="O30">
+        <v>100</v>
+      </c>
+      <c r="P30">
+        <v>300</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
       <c r="B31" t="s">
         <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>157</v>
-      </c>
-      <c r="D31" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>23</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>24</v>
       </c>
-      <c r="G31">
-        <f t="shared" ref="G31" si="17">$D$4</f>
+      <c r="H31">
+        <f t="shared" ref="H31" si="17">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>6</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <f t="shared" si="16"/>
         <v>0.25</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <f t="shared" si="3"/>
         <v>2032</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31">
+        <v>150</v>
+      </c>
+      <c r="O31">
+        <v>100</v>
+      </c>
+      <c r="P31">
+        <v>300</v>
+      </c>
+      <c r="Q31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -5200,164 +5528,221 @@
         <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>158</v>
-      </c>
-      <c r="D32" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>12</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>5</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>2018</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I32" t="s">
-        <v>80</v>
-      </c>
       <c r="J32" t="s">
         <v>80</v>
       </c>
-      <c r="K32">
+      <c r="K32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L32">
         <v>2020</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32">
+        <v>150</v>
+      </c>
+      <c r="O32">
+        <v>100</v>
+      </c>
+      <c r="P32">
+        <v>300</v>
+      </c>
+      <c r="Q32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
       <c r="B33" t="s">
         <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>159</v>
-      </c>
-      <c r="D33" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>14</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>15</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>2021</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>6</v>
       </c>
-      <c r="J33">
-        <f t="shared" ref="J33:J37" si="18">$D$3</f>
+      <c r="K33">
+        <f t="shared" ref="K33:K37" si="18">$E$3</f>
         <v>0.25</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <f t="shared" si="3"/>
         <v>2029</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="N33">
+        <v>150</v>
+      </c>
+      <c r="O33">
+        <v>100</v>
+      </c>
+      <c r="P33">
+        <v>300</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
       <c r="B34" t="s">
         <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>160</v>
-      </c>
-      <c r="D34" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>17</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>15</v>
       </c>
-      <c r="G34">
-        <f t="shared" ref="G34:G35" si="19">$D$4</f>
+      <c r="H34">
+        <f t="shared" ref="H34:H35" si="19">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>6</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <f t="shared" si="18"/>
         <v>0.25</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <f t="shared" si="3"/>
         <v>2032</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34">
+        <v>150</v>
+      </c>
+      <c r="O34">
+        <v>100</v>
+      </c>
+      <c r="P34">
+        <v>300</v>
+      </c>
+      <c r="Q34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
       <c r="B35" t="s">
         <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="D35" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" t="s">
         <v>11</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>12</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>5</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <f t="shared" si="19"/>
         <v>2024</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>6</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <f t="shared" si="18"/>
         <v>0.25</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <f t="shared" si="3"/>
         <v>2032</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="N35">
+        <v>150</v>
+      </c>
+      <c r="O35">
+        <v>100</v>
+      </c>
+      <c r="P35">
+        <v>300</v>
+      </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -5365,81 +5750,108 @@
         <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>90</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>5</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>2021</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>2</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <f t="shared" si="18"/>
         <v>0.25</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <f t="shared" si="3"/>
         <v>2026</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="N36">
+        <v>150</v>
+      </c>
+      <c r="O36">
+        <v>100</v>
+      </c>
+      <c r="P36">
+        <v>300</v>
+      </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
       <c r="B37" t="s">
         <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D37" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" t="s">
         <v>3</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>4</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>5</v>
       </c>
-      <c r="G37">
-        <f t="shared" ref="G37" si="20">$D$4</f>
+      <c r="H37">
+        <f t="shared" ref="H37" si="20">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>6</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <f t="shared" si="18"/>
         <v>0.25</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <f t="shared" si="3"/>
         <v>2032</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="N37">
+        <v>150</v>
+      </c>
+      <c r="O37">
+        <v>100</v>
+      </c>
+      <c r="P37">
+        <v>300</v>
+      </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -5447,84 +5859,108 @@
         <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>164</v>
-      </c>
-      <c r="E38" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" t="s">
+        <v>163</v>
+      </c>
+      <c r="F38" t="s">
         <v>111</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>112</v>
       </c>
-      <c r="G38">
-        <f t="shared" ref="G38:G39" si="21">$D$4</f>
+      <c r="H38">
+        <f t="shared" ref="H38:H39" si="21">$E$4</f>
         <v>2024</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>0</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>3</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>0</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <f t="shared" si="3"/>
         <v>2027</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38">
+        <v>150</v>
+      </c>
+      <c r="O38">
+        <v>100</v>
+      </c>
+      <c r="P38">
+        <v>300</v>
+      </c>
+      <c r="Q38" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" t="s">
         <v>131</v>
       </c>
-      <c r="B39" t="s">
-        <v>132</v>
-      </c>
       <c r="C39" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D39" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="E39" t="s">
         <v>133</v>
       </c>
       <c r="F39" t="s">
+        <v>132</v>
+      </c>
+      <c r="G39" t="s">
         <v>15</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <f t="shared" si="21"/>
         <v>2024</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>3</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>2</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>0.25</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <f t="shared" si="3"/>
         <v>2028</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M39" t="s">
-        <v>169</v>
+      <c r="N39">
+        <v>150</v>
+      </c>
+      <c r="O39">
+        <v>100</v>
+      </c>
+      <c r="P39">
+        <v>300</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -5532,503 +5968,617 @@
         <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F40" t="s">
-        <v>126</v>
-      </c>
-      <c r="G40">
-        <f>$D$4+$D$5</f>
+        <v>121</v>
+      </c>
+      <c r="G40" t="s">
+        <v>125</v>
+      </c>
+      <c r="H40">
+        <f>$E$4+$E$5</f>
         <v>2025</v>
       </c>
-      <c r="H40">
-        <f>$D$6+$D$7</f>
+      <c r="I40">
+        <f>$E$6+$E$7</f>
         <v>5</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>1</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>0.25</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M40" t="s">
-        <v>136</v>
+      <c r="N40">
+        <v>150</v>
+      </c>
+      <c r="O40">
+        <v>100</v>
+      </c>
+      <c r="P40">
+        <v>300</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>114</v>
+      </c>
       <c r="B41" t="s">
         <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="D41" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="E41" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F41" t="s">
-        <v>126</v>
-      </c>
-      <c r="G41">
-        <f>$D$4+$D$5</f>
+        <v>121</v>
+      </c>
+      <c r="G41" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41">
+        <f>$E$4+$E$5</f>
         <v>2025</v>
       </c>
-      <c r="H41">
-        <f t="shared" ref="H41:H42" si="22">$D$6+$D$7</f>
+      <c r="I41">
+        <f t="shared" ref="I41:I42" si="22">$E$6+$E$7</f>
         <v>5</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>1</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>0.25</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M41" t="s">
-        <v>136</v>
+      <c r="N41">
+        <v>150</v>
+      </c>
+      <c r="O41">
+        <v>100</v>
+      </c>
+      <c r="P41">
+        <v>300</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>114</v>
+      </c>
       <c r="B42" t="s">
         <v>117</v>
       </c>
       <c r="C42" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E42" t="s">
+        <v>128</v>
+      </c>
+      <c r="F42" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" t="s">
         <v>125</v>
       </c>
-      <c r="F42" t="s">
-        <v>126</v>
-      </c>
-      <c r="G42">
-        <f>$D$4+$D$5</f>
+      <c r="H42">
+        <f>$E$4+$E$5</f>
         <v>2025</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <f t="shared" si="22"/>
         <v>5</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>1</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>0.25</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M42" t="s">
+      <c r="N42">
+        <v>150</v>
+      </c>
+      <c r="O42">
+        <v>100</v>
+      </c>
+      <c r="P42">
+        <v>300</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" t="s">
+        <v>67</v>
+      </c>
+      <c r="H43">
+        <v>2031</v>
+      </c>
+      <c r="I43">
+        <f>$E$7</f>
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>0.25</v>
+      </c>
+      <c r="L43">
+        <f t="shared" ref="L43:L44" si="23">ROUNDDOWN(H43+I43+J43*(1-K43),0)</f>
+        <v>2032</v>
+      </c>
+      <c r="M43">
+        <f t="shared" ref="M43:M44" si="24">L43-H43</f>
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>150</v>
+      </c>
+      <c r="O43">
+        <v>100</v>
+      </c>
+      <c r="P43">
+        <v>300</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43" t="s">
-        <v>154</v>
-      </c>
-      <c r="D43" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" t="s">
-        <v>22</v>
-      </c>
-      <c r="F43" t="s">
-        <v>67</v>
-      </c>
-      <c r="G43">
-        <v>2031</v>
-      </c>
-      <c r="H43">
-        <f>$D$7</f>
+      <c r="C44" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" t="s">
+        <v>145</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44">
+        <v>2030</v>
+      </c>
+      <c r="I44">
+        <f t="shared" ref="I44:I45" si="25">$E$7</f>
         <v>1</v>
       </c>
-      <c r="I43">
+      <c r="J44">
         <v>1</v>
       </c>
-      <c r="J43">
+      <c r="K44">
         <v>0.25</v>
       </c>
-      <c r="K43">
-        <f t="shared" ref="K43:K44" si="23">ROUNDDOWN(G43+H43+I43*(1-J43),0)</f>
-        <v>2032</v>
-      </c>
-      <c r="L43">
-        <f t="shared" ref="L43:L44" si="24">K43-G43</f>
-        <v>1</v>
-      </c>
-      <c r="M43" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>137</v>
-      </c>
-      <c r="C44" t="s">
-        <v>146</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" t="s">
-        <v>8</v>
-      </c>
-      <c r="F44" t="s">
-        <v>5</v>
-      </c>
-      <c r="G44">
-        <v>2030</v>
-      </c>
-      <c r="H44">
-        <f t="shared" ref="H44:H45" si="25">$D$7</f>
-        <v>1</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-      <c r="J44">
-        <v>0.25</v>
-      </c>
-      <c r="K44">
+      <c r="L44">
         <f t="shared" si="23"/>
         <v>2031</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <f t="shared" si="24"/>
         <v>1</v>
       </c>
-      <c r="M44" t="s">
-        <v>136</v>
+      <c r="N44">
+        <v>150</v>
+      </c>
+      <c r="O44">
+        <v>100</v>
+      </c>
+      <c r="P44">
+        <v>300</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C45" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" t="s">
         <v>18</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>19</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>15</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>2029</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>1</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>0.25</v>
       </c>
-      <c r="K45">
-        <f t="shared" ref="K45" si="26">ROUNDDOWN(G45+H45+I45*(1-J45),0)</f>
+      <c r="L45">
+        <f t="shared" ref="L45" si="26">ROUNDDOWN(H45+I45+J45*(1-K45),0)</f>
         <v>2030</v>
       </c>
-      <c r="L45">
-        <f t="shared" ref="L45" si="27">K45-G45</f>
+      <c r="M45">
+        <f t="shared" ref="M45" si="27">L45-H45</f>
         <v>1</v>
       </c>
-      <c r="M45" t="s">
-        <v>136</v>
+      <c r="N45">
+        <v>150</v>
+      </c>
+      <c r="O45">
+        <v>100</v>
+      </c>
+      <c r="P45">
+        <v>300</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>174</v>
+      </c>
+      <c r="B46" t="s">
         <v>118</v>
       </c>
-      <c r="B46" t="s">
-        <v>119</v>
-      </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D46" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" t="s">
+        <v>137</v>
+      </c>
+      <c r="F46" t="s">
         <v>138</v>
       </c>
-      <c r="E46" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>67</v>
       </c>
-      <c r="G46">
-        <f>$D$4+$D$5</f>
+      <c r="H46">
+        <f>$E$4+$E$5</f>
         <v>2025</v>
       </c>
-      <c r="H46">
-        <f>$D$6</f>
+      <c r="I46">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>3</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>0.25</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <f t="shared" si="3"/>
         <v>2031</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M46" t="s">
-        <v>141</v>
+      <c r="N46">
+        <v>150</v>
+      </c>
+      <c r="O46">
+        <v>100</v>
+      </c>
+      <c r="P46">
+        <v>300</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>175</v>
+      </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C47" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="D47" t="s">
+        <v>153</v>
+      </c>
+      <c r="E47" t="s">
         <v>21</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>22</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>67</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>2024</v>
       </c>
-      <c r="H47">
-        <f>$D$6</f>
+      <c r="I47">
+        <f>$E$6</f>
         <v>4</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>3</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>0.25</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M47" t="s">
-        <v>141</v>
+      <c r="N47">
+        <v>150</v>
+      </c>
+      <c r="O47">
+        <v>100</v>
+      </c>
+      <c r="P47">
+        <v>300</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H52" s="6" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I52" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H53" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I53" s="8">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I53" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J53" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H54" s="7" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I54" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I54" s="8">
+      <c r="J54" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H55" s="7" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I55" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="I55" s="8">
+      <c r="J55" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H56" s="7" t="s">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I56" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I56" s="8">
+      <c r="J56" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H57" s="7" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I57" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I57" s="8">
+      <c r="J57" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H58" s="7" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I58" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I58" s="8">
+      <c r="J58" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H59" s="7" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I59" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I59" s="8">
+      <c r="J59" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H60" s="7" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I60" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I60" s="8">
+      <c r="J60" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H61" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I61" s="8">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I61" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="J61" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H62" s="7" t="s">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I62" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I62" s="8">
+      <c r="J62" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H63" s="7" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I63" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I63" s="8">
+      <c r="J63" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H64" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I64" s="8">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I64" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J64" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.35">
-      <c r="H65" s="7" t="s">
+    <row r="65" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I65" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I65" s="8">
+      <c r="J65" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.35">
-      <c r="H66" s="7" t="s">
+    <row r="66" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I66" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I66" s="8">
+      <c r="J66" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.35">
-      <c r="H67" s="7" t="s">
+    <row r="67" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I67" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I67" s="8">
+      <c r="J67" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.35">
-      <c r="H68" s="7" t="s">
+    <row r="68" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I68" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I68" s="8">
+      <c r="J68" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.35">
-      <c r="H69" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I69" s="8">
+    <row r="69" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I69" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J69" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.35">
-      <c r="H70" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="I70" s="8">
+    <row r="70" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I70" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="J70" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.35">
-      <c r="H71" s="7" t="s">
+    <row r="71" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I71" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="I71" s="8">
+      <c r="J71" s="8">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E10:E47" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
+  <autoFilter ref="F10:F47" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
Update factory specs (announced and generic) in port_scenarios input sheets
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_max.xlsx
+++ b/fabrication_ports/ports_scenario_max.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAD4956-A064-4F78-AC46-0E9F58568380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFFF17E-8D29-4E87-B0C9-593414AB4736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4178,8 +4178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10:P47"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11:P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4384,10 +4384,10 @@
         <v>150</v>
       </c>
       <c r="O11">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="P11">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
@@ -4439,10 +4439,10 @@
         <v>150</v>
       </c>
       <c r="O12">
-        <v>100</v>
+        <v>275</v>
       </c>
       <c r="P12">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="Q12" t="s">
         <v>44</v>
@@ -4497,10 +4497,10 @@
         <v>150</v>
       </c>
       <c r="O13">
-        <v>100</v>
+        <v>275</v>
       </c>
       <c r="P13">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="Q13" t="s">
         <v>44</v>
@@ -4555,10 +4555,10 @@
         <v>150</v>
       </c>
       <c r="O14">
-        <v>100</v>
+        <v>275</v>
       </c>
       <c r="P14">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="Q14" t="s">
         <v>48</v>
@@ -4613,10 +4613,10 @@
         <v>150</v>
       </c>
       <c r="O15">
-        <v>100</v>
+        <v>275</v>
       </c>
       <c r="P15">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
@@ -4670,7 +4670,7 @@
         <v>100</v>
       </c>
       <c r="P16">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="Q16" t="s">
         <v>96</v>
@@ -4727,7 +4727,7 @@
         <v>100</v>
       </c>
       <c r="P17">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="Q17" t="s">
         <v>96</v>
@@ -4785,7 +4785,7 @@
         <v>100</v>
       </c>
       <c r="P18">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
@@ -4838,7 +4838,7 @@
         <v>100</v>
       </c>
       <c r="P19">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
@@ -4888,7 +4888,7 @@
         <v>150</v>
       </c>
       <c r="O20">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="P20">
         <v>300</v>
@@ -4949,7 +4949,7 @@
         <v>100</v>
       </c>
       <c r="P21">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="Q21" t="s">
         <v>58</v>
@@ -5007,7 +5007,7 @@
         <v>100</v>
       </c>
       <c r="P22">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="Q22" t="s">
         <v>60</v>
@@ -5065,7 +5065,7 @@
         <v>100</v>
       </c>
       <c r="P23">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
@@ -5118,7 +5118,7 @@
         <v>100</v>
       </c>
       <c r="P24">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="Q24" t="s">
         <v>55</v>
@@ -5230,10 +5230,10 @@
         <v>150</v>
       </c>
       <c r="O26">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="P26">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="Q26" t="s">
         <v>68</v>
@@ -5285,10 +5285,10 @@
         <v>150</v>
       </c>
       <c r="O27">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="P27">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="Q27" t="s">
         <v>107</v>
@@ -5344,7 +5344,7 @@
         <v>100</v>
       </c>
       <c r="P28">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="Q28" t="s">
         <v>55</v>
@@ -5456,10 +5456,10 @@
         <v>150</v>
       </c>
       <c r="O30">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="P30">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
@@ -5511,10 +5511,10 @@
         <v>150</v>
       </c>
       <c r="O31">
-        <v>100</v>
+        <v>850</v>
       </c>
       <c r="P31">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="Q31" t="s">
         <v>76</v>
@@ -5566,10 +5566,10 @@
         <v>150</v>
       </c>
       <c r="O32">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P32">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="Q32" t="s">
         <v>81</v>
@@ -5623,10 +5623,10 @@
         <v>150</v>
       </c>
       <c r="O33">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P33">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -5678,10 +5678,10 @@
         <v>150</v>
       </c>
       <c r="O34">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="P34">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="Q34" t="s">
         <v>84</v>
@@ -5736,10 +5736,10 @@
         <v>150</v>
       </c>
       <c r="O35">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="P35">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -5790,10 +5790,10 @@
         <v>150</v>
       </c>
       <c r="O36">
-        <v>100</v>
+        <v>60000</v>
       </c>
       <c r="P36">
-        <v>300</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -5845,10 +5845,10 @@
         <v>150</v>
       </c>
       <c r="O37">
-        <v>100</v>
+        <v>1000000</v>
       </c>
       <c r="P37">
-        <v>300</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -5895,10 +5895,10 @@
         <v>150</v>
       </c>
       <c r="O38">
+        <v>700</v>
+      </c>
+      <c r="P38">
         <v>100</v>
-      </c>
-      <c r="P38">
-        <v>300</v>
       </c>
       <c r="Q38" t="s">
         <v>113</v>
@@ -5951,10 +5951,10 @@
         <v>150</v>
       </c>
       <c r="O39">
+        <v>5000</v>
+      </c>
+      <c r="P39">
         <v>100</v>
-      </c>
-      <c r="P39">
-        <v>300</v>
       </c>
       <c r="Q39" t="s">
         <v>168</v>
@@ -6008,10 +6008,10 @@
         <v>150</v>
       </c>
       <c r="O40">
+        <v>50</v>
+      </c>
+      <c r="P40">
         <v>100</v>
-      </c>
-      <c r="P40">
-        <v>300</v>
       </c>
       <c r="Q40" t="s">
         <v>135</v>
@@ -6065,10 +6065,10 @@
         <v>150</v>
       </c>
       <c r="O41">
+        <v>50</v>
+      </c>
+      <c r="P41">
         <v>100</v>
-      </c>
-      <c r="P41">
-        <v>300</v>
       </c>
       <c r="Q41" t="s">
         <v>135</v>
@@ -6122,10 +6122,10 @@
         <v>150</v>
       </c>
       <c r="O42">
+        <v>50</v>
+      </c>
+      <c r="P42">
         <v>100</v>
-      </c>
-      <c r="P42">
-        <v>300</v>
       </c>
       <c r="Q42" t="s">
         <v>135</v>
@@ -6178,10 +6178,10 @@
         <v>150</v>
       </c>
       <c r="O43">
+        <v>50</v>
+      </c>
+      <c r="P43">
         <v>100</v>
-      </c>
-      <c r="P43">
-        <v>300</v>
       </c>
       <c r="Q43" t="s">
         <v>135</v>
@@ -6234,10 +6234,10 @@
         <v>150</v>
       </c>
       <c r="O44">
+        <v>50</v>
+      </c>
+      <c r="P44">
         <v>100</v>
-      </c>
-      <c r="P44">
-        <v>300</v>
       </c>
       <c r="Q44" t="s">
         <v>135</v>
@@ -6290,10 +6290,10 @@
         <v>150</v>
       </c>
       <c r="O45">
+        <v>50</v>
+      </c>
+      <c r="P45">
         <v>100</v>
-      </c>
-      <c r="P45">
-        <v>300</v>
       </c>
       <c r="Q45" t="s">
         <v>135</v>
@@ -6347,10 +6347,10 @@
         <v>150</v>
       </c>
       <c r="O46">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="P46">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="Q46" t="s">
         <v>140</v>
@@ -6403,10 +6403,10 @@
         <v>150</v>
       </c>
       <c r="O47">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="P47">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="Q47" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
Update scenarios based on cable and blade reviewer feedback
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_max.xlsx
+++ b/fabrication_ports/ports_scenario_max.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F3B2D6-CDCA-446B-92F5-ECFF81917748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548F2646-EFC9-4E61-AFAE-426914BF7BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="179">
   <si>
     <t>Port</t>
   </si>
@@ -572,13 +572,16 @@
   </si>
   <si>
     <t>Facility cost</t>
+  </si>
+  <si>
+    <t>HVDC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,6 +607,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -659,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -677,6 +686,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4179,7 +4189,7 @@
   <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4384,10 +4394,10 @@
         <v>150</v>
       </c>
       <c r="O11">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="P11">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
@@ -4439,7 +4449,7 @@
         <v>150</v>
       </c>
       <c r="O12">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="P12">
         <v>250</v>
@@ -4497,7 +4507,7 @@
         <v>150</v>
       </c>
       <c r="O13">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="P13">
         <v>250</v>
@@ -4555,7 +4565,7 @@
         <v>150</v>
       </c>
       <c r="O14">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="P14">
         <v>250</v>
@@ -4613,7 +4623,7 @@
         <v>150</v>
       </c>
       <c r="O15">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="P15">
         <v>250</v>
@@ -5511,10 +5521,10 @@
         <v>150</v>
       </c>
       <c r="O31">
-        <v>850</v>
+        <v>500</v>
       </c>
       <c r="P31">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="Q31" t="s">
         <v>76</v>
@@ -5622,7 +5632,7 @@
       <c r="N33">
         <v>150</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="9">
         <v>200</v>
       </c>
       <c r="P33">
@@ -5677,11 +5687,11 @@
       <c r="N34">
         <v>150</v>
       </c>
-      <c r="O34">
-        <v>500</v>
+      <c r="O34" s="9">
+        <v>200</v>
       </c>
       <c r="P34">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="Q34" t="s">
         <v>84</v>
@@ -5735,11 +5745,14 @@
       <c r="N35">
         <v>150</v>
       </c>
-      <c r="O35">
-        <v>500</v>
+      <c r="O35" s="9">
+        <v>600</v>
       </c>
       <c r="P35">
-        <v>200</v>
+        <v>400</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -5789,7 +5802,7 @@
       <c r="N36">
         <v>150</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="9">
         <v>60000</v>
       </c>
       <c r="P36">

</xml_diff>

<commit_message>
Adding plot for number of facilities per state
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_max.xlsx
+++ b/fabrication_ports/ports_scenario_max.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548F2646-EFC9-4E61-AFAE-426914BF7BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355B551C-DA81-41A6-82DF-350FCAE45E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId2"/>
+    <pivotCache cacheId="1" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -668,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -685,7 +685,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1516,43 +1515,15 @@
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -1627,7 +1598,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1837,20 +1810,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of facilities</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1885,6 +1899,7 @@
         <c:crossAx val="854290856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1894,37 +1909,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1970,9 +1954,6 @@
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
       <c14:pivotOptions>
         <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
@@ -3772,7 +3753,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="I52:J71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -4188,8 +4169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5632,7 +5613,7 @@
       <c r="N33">
         <v>150</v>
       </c>
-      <c r="O33" s="9">
+      <c r="O33" s="8">
         <v>200</v>
       </c>
       <c r="P33">
@@ -5687,7 +5668,7 @@
       <c r="N34">
         <v>150</v>
       </c>
-      <c r="O34" s="9">
+      <c r="O34" s="8">
         <v>200</v>
       </c>
       <c r="P34">
@@ -5745,7 +5726,7 @@
       <c r="N35">
         <v>150</v>
       </c>
-      <c r="O35" s="9">
+      <c r="O35" s="8">
         <v>600</v>
       </c>
       <c r="P35">
@@ -5802,7 +5783,7 @@
       <c r="N36">
         <v>150</v>
       </c>
-      <c r="O36" s="9">
+      <c r="O36" s="8">
         <v>60000</v>
       </c>
       <c r="P36">
@@ -6442,7 +6423,7 @@
       <c r="I53" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J53" s="8">
+      <c r="J53">
         <v>4</v>
       </c>
     </row>
@@ -6450,7 +6431,7 @@
       <c r="I54" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J54" s="8">
+      <c r="J54">
         <v>1</v>
       </c>
     </row>
@@ -6458,7 +6439,7 @@
       <c r="I55" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="J55" s="8">
+      <c r="J55">
         <v>1</v>
       </c>
     </row>
@@ -6466,7 +6447,7 @@
       <c r="I56" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J56" s="8">
+      <c r="J56">
         <v>3</v>
       </c>
     </row>
@@ -6474,7 +6455,7 @@
       <c r="I57" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J57" s="8">
+      <c r="J57">
         <v>2</v>
       </c>
     </row>
@@ -6482,7 +6463,7 @@
       <c r="I58" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J58" s="8">
+      <c r="J58">
         <v>3</v>
       </c>
     </row>
@@ -6490,7 +6471,7 @@
       <c r="I59" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J59" s="8">
+      <c r="J59">
         <v>2</v>
       </c>
     </row>
@@ -6498,7 +6479,7 @@
       <c r="I60" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J60" s="8">
+      <c r="J60">
         <v>2</v>
       </c>
     </row>
@@ -6506,7 +6487,7 @@
       <c r="I61" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J61" s="8">
+      <c r="J61">
         <v>1</v>
       </c>
     </row>
@@ -6514,7 +6495,7 @@
       <c r="I62" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J62" s="8">
+      <c r="J62">
         <v>4</v>
       </c>
     </row>
@@ -6522,7 +6503,7 @@
       <c r="I63" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J63" s="8">
+      <c r="J63">
         <v>4</v>
       </c>
     </row>
@@ -6530,7 +6511,7 @@
       <c r="I64" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J64" s="8">
+      <c r="J64">
         <v>2</v>
       </c>
     </row>
@@ -6538,7 +6519,7 @@
       <c r="I65" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="J65" s="8">
+      <c r="J65">
         <v>1</v>
       </c>
     </row>
@@ -6546,7 +6527,7 @@
       <c r="I66" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J66" s="8">
+      <c r="J66">
         <v>2</v>
       </c>
     </row>
@@ -6554,7 +6535,7 @@
       <c r="I67" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J67" s="8">
+      <c r="J67">
         <v>2</v>
       </c>
     </row>
@@ -6562,7 +6543,7 @@
       <c r="I68" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J68" s="8">
+      <c r="J68">
         <v>2</v>
       </c>
     </row>
@@ -6570,7 +6551,7 @@
       <c r="I69" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="J69" s="8">
+      <c r="J69">
         <v>1</v>
       </c>
     </row>
@@ -6578,7 +6559,7 @@
       <c r="I70" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="J70" s="8">
+      <c r="J70">
         <v>2</v>
       </c>
     </row>
@@ -6586,7 +6567,7 @@
       <c r="I71" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="J71" s="8">
+      <c r="J71">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added monopile facility.  Removed 4x semisub facilities.  Removed mooring rope.  Updated port upgrade costs
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_max.xlsx
+++ b/fabrication_ports/ports_scenario_max.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355B551C-DA81-41A6-82DF-350FCAE45E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD773CC-8815-4321-9276-B01C5D778056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$F$10:$F$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$F$10:$F$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="172">
   <si>
     <t>Port</t>
   </si>
@@ -388,18 +388,12 @@
     <t>Semisubmersible 1</t>
   </si>
   <si>
-    <t>Semisubmersible 2</t>
-  </si>
-  <si>
     <t>Semisubmersible 3</t>
   </si>
   <si>
     <t>Mooring chain 1</t>
   </si>
   <si>
-    <t>Mooring rope 1</t>
-  </si>
-  <si>
     <t>Blade 4</t>
   </si>
   <si>
@@ -421,9 +415,6 @@
     <t>TBD - Humboldt</t>
   </si>
   <si>
-    <t>TBD - Central Coast</t>
-  </si>
-  <si>
     <t>TBD - Coos Bay</t>
   </si>
   <si>
@@ -442,24 +433,15 @@
     <t>Schiller Newington, Portsmouth</t>
   </si>
   <si>
-    <t>Semisubmersible 4</t>
-  </si>
-  <si>
     <t>Assembly port</t>
   </si>
   <si>
-    <t>Semisubmersible 5</t>
-  </si>
-  <si>
     <t>TBD - TX</t>
   </si>
   <si>
     <t>TX</t>
   </si>
   <si>
-    <t>Semisubmersible 6</t>
-  </si>
-  <si>
     <t>Service WC and EC</t>
   </si>
   <si>
@@ -535,9 +517,6 @@
     <t>Portsmouth, NH</t>
   </si>
   <si>
-    <t>Central Coast, CA</t>
-  </si>
-  <si>
     <t>TX port, TX</t>
   </si>
   <si>
@@ -565,9 +544,6 @@
     <t>Mooring chain</t>
   </si>
   <si>
-    <t>Mooring rope</t>
-  </si>
-  <si>
     <t>Production capacity</t>
   </si>
   <si>
@@ -575,6 +551,9 @@
   </si>
   <si>
     <t>HVDC</t>
+  </si>
+  <si>
+    <t>Monopile 1</t>
   </si>
 </sst>
 </file>
@@ -792,9 +771,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$11:$B$47</c:f>
+              <c:f>'Avg Demand Scenario'!$B$11:$B$43</c:f>
               <c:strCache>
-                <c:ptCount val="37"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -841,80 +820,68 @@
                   <c:v>US Wind</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>Monopile 1</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>Jacket 1</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>GBF 1</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Smulders</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Transition piece 1</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Hellenic</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Array cable 1</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Nexans</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Prysmian</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Export cable 1</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Export cable 2</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Nucor</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Steel plate 1</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>Casting 1</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>Flange 1</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>Semisubmersible 1</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Semisubmersible 2</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>Semisubmersible 3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Semisubmersible 4</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Semisubmersible 5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Semisubmersible 6</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>Mooring chain 1</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Mooring rope 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$H$11:$H$47</c:f>
+              <c:f>'Avg Demand Scenario'!$H$11:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>2021</c:v>
                 </c:pt>
@@ -964,37 +931,37 @@
                   <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2025</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>2021</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>2024</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>2021</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>2024</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>2018</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>2024</c:v>
@@ -1003,7 +970,7 @@
                   <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2025</c:v>
+                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>2025</c:v>
@@ -1012,19 +979,7 @@
                   <c:v>2025</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2031</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2030</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2029</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1050,9 +1005,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$11:$B$47</c:f>
+              <c:f>'Avg Demand Scenario'!$B$11:$B$43</c:f>
               <c:strCache>
-                <c:ptCount val="37"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>SGRE</c:v>
                 </c:pt>
@@ -1099,80 +1054,68 @@
                   <c:v>US Wind</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>Monopile 1</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>Jacket 1</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>GBF 1</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Smulders</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Transition piece 1</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Hellenic</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Array cable 1</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Nexans</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Prysmian</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Export cable 1</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Export cable 2</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Nucor</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Steel plate 1</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>Casting 1</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>Flange 1</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>Semisubmersible 1</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Semisubmersible 2</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>Semisubmersible 3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Semisubmersible 4</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Semisubmersible 5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Semisubmersible 6</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>Mooring chain 1</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Mooring rope 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$M$11:$M$47</c:f>
+              <c:f>'Avg Demand Scenario'!$M$11:$M$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -1219,28 +1162,28 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>8</c:v>
@@ -1249,19 +1192,19 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>5</c:v>
@@ -1270,18 +1213,6 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="36">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1587,7 +1518,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$J$52</c:f>
+              <c:f>'Avg Demand Scenario'!$J$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1610,7 +1541,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$I$53:$I$71</c:f>
+              <c:f>'Avg Demand Scenario'!$I$49:$I$67</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -1672,7 +1603,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$J$53:$J$71</c:f>
+              <c:f>'Avg Demand Scenario'!$J$49:$J$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -3060,13 +2991,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30254</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>58177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>244928</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3096,13 +3027,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>898921</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>75008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>2458640</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>151208</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3134,7 +3065,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44771.490716435183" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A10:M47" sheet="Avg Demand Scenario"/>
+    <worksheetSource ref="A10:M43" sheet="Avg Demand Scenario"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Component" numFmtId="0">
@@ -3754,7 +3685,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
-  <location ref="I52:J71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="I48:J67" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -4167,10 +4098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4222,7 +4153,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -4244,7 +4175,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -4282,10 +4213,10 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>0</v>
@@ -4315,13 +4246,13 @@
         <v>39</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>40</v>
@@ -4335,10 +4266,10 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -4389,10 +4320,10 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
@@ -4423,7 +4354,7 @@
         <v>2031</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12:M47" si="1">L12-H12</f>
+        <f t="shared" ref="M12:M43" si="1">L12-H12</f>
         <v>7</v>
       </c>
       <c r="N12">
@@ -4447,10 +4378,10 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>20</v>
@@ -4477,7 +4408,7 @@
         <v>0.25</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13:L47" si="3">ROUNDDOWN(H13+I13+J13*(1-K13),0)</f>
+        <f t="shared" ref="L13:L43" si="3">ROUNDDOWN(H13+I13+J13*(1-K13),0)</f>
         <v>2031</v>
       </c>
       <c r="M13">
@@ -4485,7 +4416,7 @@
         <v>7</v>
       </c>
       <c r="N13">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="O13">
         <v>225</v>
@@ -4505,10 +4436,10 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>47</v>
@@ -4560,22 +4491,22 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H15">
         <f>$E$4+$E$5</f>
@@ -4601,7 +4532,7 @@
         <v>8</v>
       </c>
       <c r="N15">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="O15">
         <v>225</v>
@@ -4618,10 +4549,10 @@
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
@@ -4675,10 +4606,10 @@
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
@@ -4732,10 +4663,10 @@
         <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>29</v>
@@ -4770,7 +4701,7 @@
         <v>7</v>
       </c>
       <c r="N18">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="O18">
         <v>100</v>
@@ -4784,22 +4715,22 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H19">
         <v>2023</v>
@@ -4823,7 +4754,7 @@
         <v>8</v>
       </c>
       <c r="N19">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="O19">
         <v>100</v>
@@ -4840,10 +4771,10 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>25</v>
@@ -4876,7 +4807,7 @@
         <v>4</v>
       </c>
       <c r="N20">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="O20">
         <v>150</v>
@@ -4896,10 +4827,10 @@
         <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>57</v>
@@ -4954,10 +4885,10 @@
         <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>18</v>
@@ -5009,22 +4940,22 @@
         <v>53</v>
       </c>
       <c r="B23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" t="s">
+        <v>119</v>
+      </c>
+      <c r="G23" t="s">
         <v>123</v>
-      </c>
-      <c r="C23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D23" t="s">
-        <v>148</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" t="s">
-        <v>121</v>
-      </c>
-      <c r="G23" t="s">
-        <v>125</v>
       </c>
       <c r="H23">
         <f>$E$4+$E$5</f>
@@ -5067,10 +4998,10 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D24" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>27</v>
@@ -5123,10 +5054,10 @@
         <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D25" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>57</v>
@@ -5148,7 +5079,7 @@
         <v>3.5</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:K26" si="12">$E$3</f>
+        <f t="shared" ref="K25:K27" si="12">$E$3</f>
         <v>0.25</v>
       </c>
       <c r="L25">
@@ -5174,28 +5105,28 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>171</v>
       </c>
       <c r="C26" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D26" t="s">
-        <v>153</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>21</v>
+        <v>139</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="H26">
-        <f t="shared" ref="H26" si="13">$E$4</f>
+        <f>E4</f>
         <v>2024</v>
       </c>
       <c r="I26">
@@ -5203,66 +5134,65 @@
         <v>4</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K26">
-        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
       <c r="L26">
-        <f>ROUNDDOWN(H26+I26+J26*(1-K26),0)</f>
-        <v>2029</v>
+        <f t="shared" si="3"/>
+        <v>2031</v>
       </c>
       <c r="M26">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N26">
         <v>150</v>
       </c>
       <c r="O26">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="P26">
-        <v>10</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>68</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>86</v>
+        <v>147</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="H27">
-        <v>2025</v>
+        <f t="shared" ref="H27" si="13">$E$4</f>
+        <v>2024</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <f>$E$6</f>
+        <v>4</v>
       </c>
       <c r="J27">
         <v>2</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0.25</v>
       </c>
       <c r="L27">
         <f>ROUNDDOWN(H27+I27+J27*(1-K27),0)</f>
@@ -5270,7 +5200,7 @@
       </c>
       <c r="M27">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N27">
         <v>150</v>
@@ -5282,63 +5212,62 @@
         <v>10</v>
       </c>
       <c r="Q27" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>25</v>
+        <v>148</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H28">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="I28">
-        <f t="shared" ref="I28:I37" si="14">$E$6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K28">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L28">
-        <f t="shared" si="3"/>
-        <v>2027</v>
+        <f>ROUNDDOWN(H28+I28+J28*(1-K28),0)</f>
+        <v>2029</v>
       </c>
       <c r="M28">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N28">
         <v>150</v>
       </c>
       <c r="O28">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="P28">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="Q28" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
@@ -5346,16 +5275,16 @@
         <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D29" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="F29" t="s">
         <v>23</v>
@@ -5364,93 +5293,95 @@
         <v>24</v>
       </c>
       <c r="H29">
-        <f t="shared" ref="H29" si="15">$E$4</f>
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="I29">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="I29:I38" si="14">$E$6</f>
         <v>4</v>
       </c>
       <c r="J29">
         <v>3</v>
       </c>
       <c r="K29">
-        <f t="shared" ref="K29:K31" si="16">$E$3</f>
         <v>0.25</v>
       </c>
       <c r="L29">
         <f t="shared" si="3"/>
-        <v>2030</v>
+        <v>2027</v>
       </c>
       <c r="M29">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="N29">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="O29">
         <v>100</v>
       </c>
       <c r="P29">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="Q29" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="C30" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F30" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G30" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="H30">
-        <v>2021</v>
+        <f t="shared" ref="H30" si="15">$E$4</f>
+        <v>2024</v>
       </c>
       <c r="I30">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="J30">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K30">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="K30:K32" si="16">$E$3</f>
         <v>0.25</v>
       </c>
       <c r="L30">
         <f t="shared" si="3"/>
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="M30">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N30">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="O30">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="P30">
-        <v>200</v>
+        <v>300</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
@@ -5458,26 +5389,25 @@
         <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G31" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31" si="17">$E$4</f>
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="I31">
         <f t="shared" si="14"/>
@@ -5492,7 +5422,7 @@
       </c>
       <c r="L31">
         <f t="shared" si="3"/>
-        <v>2032</v>
+        <v>2029</v>
       </c>
       <c r="M31">
         <f t="shared" si="1"/>
@@ -5502,68 +5432,68 @@
         <v>150</v>
       </c>
       <c r="O31">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="P31">
-        <v>400</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>76</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G32" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="H32">
-        <v>2018</v>
+        <f t="shared" ref="H32" si="17">$E$4</f>
+        <v>2024</v>
       </c>
       <c r="I32">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="J32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K32" t="s">
-        <v>80</v>
+      <c r="J32">
+        <v>6</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="16"/>
+        <v>0.25</v>
       </c>
       <c r="L32">
-        <v>2020</v>
+        <f t="shared" si="3"/>
+        <v>2032</v>
       </c>
       <c r="M32">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N32">
         <v>150</v>
       </c>
       <c r="O32">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="P32">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="Q32" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -5571,53 +5501,54 @@
         <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D33" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H33">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="I33">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="J33">
-        <v>6</v>
-      </c>
-      <c r="K33">
-        <f t="shared" ref="K33:K37" si="18">$E$3</f>
-        <v>0.25</v>
+      <c r="J33" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" t="s">
+        <v>80</v>
       </c>
       <c r="L33">
-        <f t="shared" si="3"/>
-        <v>2029</v>
+        <v>2020</v>
       </c>
       <c r="M33">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N33">
-        <v>150</v>
-      </c>
-      <c r="O33" s="8">
+        <v>50</v>
+      </c>
+      <c r="O33">
         <v>200</v>
       </c>
       <c r="P33">
         <v>200</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -5625,26 +5556,25 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D34" t="s">
-        <v>159</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>16</v>
+        <v>152</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G34" t="s">
         <v>15</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H35" si="19">$E$4</f>
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="I34">
         <f t="shared" si="14"/>
@@ -5654,12 +5584,12 @@
         <v>6</v>
       </c>
       <c r="K34">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="K34:K38" si="18">$E$3</f>
         <v>0.25</v>
       </c>
       <c r="L34">
         <f t="shared" si="3"/>
-        <v>2032</v>
+        <v>2029</v>
       </c>
       <c r="M34">
         <f t="shared" si="1"/>
@@ -5672,10 +5602,7 @@
         <v>200</v>
       </c>
       <c r="P34">
-        <v>400</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -5683,25 +5610,25 @@
         <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
+        <v>153</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G35" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H35">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="H35:H36" si="19">$E$4</f>
         <v>2024</v>
       </c>
       <c r="I35">
@@ -5727,46 +5654,47 @@
         <v>150</v>
       </c>
       <c r="O35" s="8">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="P35">
         <v>400</v>
       </c>
       <c r="Q35" t="s">
-        <v>178</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>89</v>
+        <v>154</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36">
-        <v>2021</v>
+        <f t="shared" si="19"/>
+        <v>2024</v>
       </c>
       <c r="I36">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="J36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K36">
         <f t="shared" si="18"/>
@@ -5774,20 +5702,23 @@
       </c>
       <c r="L36">
         <f t="shared" si="3"/>
-        <v>2026</v>
+        <v>2032</v>
       </c>
       <c r="M36">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N36">
         <v>150</v>
       </c>
       <c r="O36" s="8">
-        <v>60000</v>
+        <v>600</v>
       </c>
       <c r="P36">
-        <v>1000</v>
+        <v>400</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -5795,33 +5726,32 @@
         <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D37" t="s">
-        <v>162</v>
-      </c>
-      <c r="E37" t="s">
-        <v>3</v>
+        <v>155</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="F37" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37" si="20">$E$4</f>
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="I37">
         <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="J37">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K37">
         <f t="shared" si="18"/>
@@ -5829,186 +5759,184 @@
       </c>
       <c r="L37">
         <f t="shared" si="3"/>
-        <v>2032</v>
+        <v>2026</v>
       </c>
       <c r="M37">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N37">
         <v>150</v>
       </c>
-      <c r="O37">
-        <v>1000000</v>
+      <c r="O37" s="8">
+        <v>60000</v>
       </c>
       <c r="P37">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D38" t="s">
-        <v>163</v>
+        <v>156</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="G38" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="H38">
-        <f t="shared" ref="H38:H39" si="21">$E$4</f>
+        <f t="shared" ref="H38" si="20">$E$4</f>
         <v>2024</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>4</v>
       </c>
       <c r="J38">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>0.25</v>
       </c>
       <c r="L38">
         <f t="shared" si="3"/>
-        <v>2027</v>
+        <v>2032</v>
       </c>
       <c r="M38">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N38">
         <v>150</v>
       </c>
       <c r="O38">
-        <v>700</v>
+        <v>1000000</v>
       </c>
       <c r="P38">
-        <v>100</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>113</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D39" t="s">
-        <v>164</v>
-      </c>
-      <c r="E39" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="F39" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="H39">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="H39:H40" si="21">$E$4</f>
         <v>2024</v>
       </c>
       <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
         <v>3</v>
       </c>
-      <c r="J39">
-        <v>2</v>
-      </c>
       <c r="K39">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L39">
         <f t="shared" si="3"/>
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="M39">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N39">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="O39">
-        <v>5000</v>
+        <v>700</v>
       </c>
       <c r="P39">
         <v>100</v>
       </c>
       <c r="Q39" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D40" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F40" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="G40" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="H40">
-        <f>$E$4+$E$5</f>
-        <v>2025</v>
+        <f t="shared" si="21"/>
+        <v>2024</v>
       </c>
       <c r="I40">
-        <f>$E$6+$E$7</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K40">
         <v>0.25</v>
       </c>
       <c r="L40">
         <f t="shared" si="3"/>
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="M40">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N40">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="O40">
-        <v>50</v>
+        <v>5000</v>
       </c>
       <c r="P40">
         <v>100</v>
       </c>
       <c r="Q40" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -6016,29 +5944,29 @@
         <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C41" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="E41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H41">
         <f>$E$4+$E$5</f>
         <v>2025</v>
       </c>
       <c r="I41">
-        <f t="shared" ref="I41:I42" si="22">$E$6+$E$7</f>
+        <f>$E$6+$E$7</f>
         <v>5</v>
       </c>
       <c r="J41">
@@ -6065,7 +5993,7 @@
         <v>100</v>
       </c>
       <c r="Q41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
@@ -6073,29 +6001,29 @@
         <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E42" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H42">
         <f>$E$4+$E$5</f>
         <v>2025</v>
       </c>
       <c r="I42">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="I42" si="22">$E$6+$E$7</f>
         <v>5</v>
       </c>
       <c r="J42">
@@ -6122,394 +6050,202 @@
         <v>100</v>
       </c>
       <c r="Q42" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D43" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E43" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
       <c r="F43" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="G43" t="s">
         <v>67</v>
       </c>
       <c r="H43">
-        <v>2031</v>
+        <f>$E$4+$E$5</f>
+        <v>2025</v>
       </c>
       <c r="I43">
-        <f>$E$7</f>
-        <v>1</v>
+        <f>$E$6</f>
+        <v>4</v>
       </c>
       <c r="J43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K43">
         <v>0.25</v>
       </c>
       <c r="L43">
-        <f t="shared" ref="L43:L44" si="23">ROUNDDOWN(H43+I43+J43*(1-K43),0)</f>
-        <v>2032</v>
+        <f t="shared" si="3"/>
+        <v>2031</v>
       </c>
       <c r="M43">
-        <f t="shared" ref="M43:M44" si="24">L43-H43</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="N43">
         <v>150</v>
       </c>
       <c r="O43">
+        <v>2000</v>
+      </c>
+      <c r="P43">
         <v>50</v>
       </c>
-      <c r="P43">
-        <v>100</v>
-      </c>
       <c r="Q43" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" t="s">
-        <v>136</v>
-      </c>
-      <c r="C44" t="s">
-        <v>173</v>
-      </c>
-      <c r="D44" t="s">
-        <v>145</v>
-      </c>
-      <c r="E44" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" t="s">
-        <v>8</v>
-      </c>
-      <c r="G44" t="s">
-        <v>5</v>
-      </c>
-      <c r="H44">
-        <v>2030</v>
-      </c>
-      <c r="I44">
-        <f t="shared" ref="I44:I45" si="25">$E$7</f>
-        <v>1</v>
-      </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-      <c r="K44">
-        <v>0.25</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="23"/>
-        <v>2031</v>
-      </c>
-      <c r="M44">
-        <f t="shared" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="N44">
-        <v>150</v>
-      </c>
-      <c r="O44">
-        <v>50</v>
-      </c>
-      <c r="P44">
-        <v>100</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>114</v>
-      </c>
-      <c r="B45" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45">
-        <v>2029</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-      <c r="K45">
-        <v>0.25</v>
-      </c>
-      <c r="L45">
-        <f t="shared" ref="L45" si="26">ROUNDDOWN(H45+I45+J45*(1-K45),0)</f>
-        <v>2030</v>
-      </c>
-      <c r="M45">
-        <f t="shared" ref="M45" si="27">L45-H45</f>
-        <v>1</v>
-      </c>
-      <c r="N45">
-        <v>150</v>
-      </c>
-      <c r="O45">
-        <v>50</v>
-      </c>
-      <c r="P45">
-        <v>100</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>174</v>
-      </c>
-      <c r="B46" t="s">
-        <v>118</v>
-      </c>
-      <c r="C46" t="s">
-        <v>173</v>
-      </c>
-      <c r="D46" t="s">
-        <v>166</v>
-      </c>
-      <c r="E46" t="s">
-        <v>137</v>
-      </c>
-      <c r="F46" t="s">
-        <v>138</v>
-      </c>
-      <c r="G46" t="s">
-        <v>67</v>
-      </c>
-      <c r="H46">
-        <f>$E$4+$E$5</f>
-        <v>2025</v>
-      </c>
-      <c r="I46">
-        <f>$E$6</f>
+      <c r="A46" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="I48" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I49" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="J49">
         <v>4</v>
       </c>
-      <c r="J46">
+    </row>
+    <row r="50" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I50" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I51" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I52" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J52">
         <v>3</v>
       </c>
-      <c r="K46">
-        <v>0.25</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="3"/>
-        <v>2031</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="53" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I53" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N46">
-        <v>150</v>
-      </c>
-      <c r="O46">
-        <v>2000</v>
-      </c>
-      <c r="P46">
-        <v>50</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>140</v>
+      <c r="J54">
+        <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>175</v>
-      </c>
-      <c r="B47" t="s">
-        <v>119</v>
-      </c>
-      <c r="C47" t="s">
-        <v>173</v>
-      </c>
-      <c r="D47" t="s">
-        <v>153</v>
-      </c>
-      <c r="E47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F47" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" t="s">
-        <v>67</v>
-      </c>
-      <c r="H47">
-        <v>2024</v>
-      </c>
-      <c r="I47">
-        <f>$E$6</f>
+    <row r="55" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I55" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I56" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I57" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I58" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J58">
         <v>4</v>
       </c>
-      <c r="J47">
-        <v>3</v>
-      </c>
-      <c r="K47">
-        <v>0.25</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="3"/>
-        <v>2030</v>
-      </c>
-      <c r="M47">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="N47">
-        <v>150</v>
-      </c>
-      <c r="O47">
-        <v>2000</v>
-      </c>
-      <c r="P47">
-        <v>50</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>140</v>
-      </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>101</v>
+    <row r="59" spans="9:10" x14ac:dyDescent="0.35">
+      <c r="I59" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J59">
+        <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I52" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="J52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I53" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J53">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I54" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I55" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I56" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J56">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I57" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I58" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J58">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I59" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I60" s="7" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="J60">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I61" s="7" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="J61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I62" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J62">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I63" s="7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J63">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I64" s="7" t="s">
-        <v>124</v>
+        <v>8</v>
       </c>
       <c r="J64">
         <v>2</v>
@@ -6517,7 +6253,7 @@
     </row>
     <row r="65" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I65" s="7" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="J65">
         <v>1</v>
@@ -6525,7 +6261,7 @@
     </row>
     <row r="66" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I66" s="7" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="J66">
         <v>2</v>
@@ -6533,46 +6269,14 @@
     </row>
     <row r="67" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I67" s="7" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="J67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I68" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I69" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="J69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I70" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="J70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="9:10" x14ac:dyDescent="0.35">
-      <c r="I71" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="J71">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F10:F47" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
+  <autoFilter ref="F10:F43" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
updated semisubmersible to floating platform
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_max.xlsx
+++ b/fabrication_ports/ports_scenario_max.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD773CC-8815-4321-9276-B01C5D778056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C5C579-0F48-465F-A076-93C3C06BEAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="176">
   <si>
     <t>Port</t>
   </si>
@@ -382,18 +382,12 @@
     <t xml:space="preserve">Doesn't need to be at a port.  Exising large foundries in OH, PA. </t>
   </si>
   <si>
-    <t>Semisubmersible</t>
-  </si>
-  <si>
-    <t>Semisubmersible 1</t>
-  </si>
-  <si>
-    <t>Semisubmersible 3</t>
-  </si>
-  <si>
     <t>Mooring chain 1</t>
   </si>
   <si>
+    <t>Mooring rope 1</t>
+  </si>
+  <si>
     <t>Blade 4</t>
   </si>
   <si>
@@ -544,6 +538,9 @@
     <t>Mooring chain</t>
   </si>
   <si>
+    <t>Mooring rope</t>
+  </si>
+  <si>
     <t>Production capacity</t>
   </si>
   <si>
@@ -554,6 +551,21 @@
   </si>
   <si>
     <t>Monopile 1</t>
+  </si>
+  <si>
+    <t>Assume relatively minor upgrades to existin industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Floating platform</t>
+  </si>
+  <si>
+    <t>Floating platform 1</t>
+  </si>
+  <si>
+    <t>Floating platform 2</t>
   </si>
 </sst>
 </file>
@@ -865,10 +877,10 @@
                   <c:v>Flange 1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Semisubmersible 1</c:v>
+                  <c:v>Floating platform 1</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Semisubmersible 3</c:v>
+                  <c:v>Floating platform 2</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>Mooring chain 1</c:v>
@@ -1099,10 +1111,10 @@
                   <c:v>Flange 1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>Semisubmersible 1</c:v>
+                  <c:v>Floating platform 1</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Semisubmersible 3</c:v>
+                  <c:v>Floating platform 2</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>Mooring chain 1</c:v>
@@ -4100,13 +4112,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
     <col min="2" max="4" width="25.1796875" customWidth="1"/>
     <col min="5" max="5" width="42.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.453125" customWidth="1"/>
@@ -4153,7 +4165,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -4175,7 +4187,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -4213,10 +4225,10 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>0</v>
@@ -4246,13 +4258,13 @@
         <v>39</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>40</v>
@@ -4266,10 +4278,10 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -4320,10 +4332,10 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
@@ -4378,10 +4390,10 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>20</v>
@@ -4436,10 +4448,10 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>47</v>
@@ -4491,22 +4503,22 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H15">
         <f>$E$4+$E$5</f>
@@ -4549,10 +4561,10 @@
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
@@ -4606,10 +4618,10 @@
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
@@ -4663,10 +4675,10 @@
         <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>29</v>
@@ -4715,22 +4727,22 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H19">
         <v>2023</v>
@@ -4771,10 +4783,10 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>25</v>
@@ -4827,10 +4839,10 @@
         <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>57</v>
@@ -4885,10 +4897,10 @@
         <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>18</v>
@@ -4940,22 +4952,22 @@
         <v>53</v>
       </c>
       <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" t="s">
         <v>121</v>
-      </c>
-      <c r="C23" t="s">
-        <v>166</v>
-      </c>
-      <c r="D23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" t="s">
-        <v>119</v>
-      </c>
-      <c r="G23" t="s">
-        <v>123</v>
       </c>
       <c r="H23">
         <f>$E$4+$E$5</f>
@@ -4998,10 +5010,10 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>27</v>
@@ -5054,10 +5066,10 @@
         <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>57</v>
@@ -5108,13 +5120,13 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -5165,10 +5177,10 @@
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>21</v>
@@ -5223,10 +5235,10 @@
         <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>86</v>
@@ -5278,10 +5290,10 @@
         <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>25</v>
@@ -5334,10 +5346,10 @@
         <v>108</v>
       </c>
       <c r="C30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>71</v>
@@ -5392,10 +5404,10 @@
         <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>57</v>
@@ -5446,10 +5458,10 @@
         <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>28</v>
@@ -5504,10 +5516,10 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>79</v>
@@ -5559,10 +5571,10 @@
         <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>13</v>
@@ -5613,10 +5625,10 @@
         <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>16</v>
@@ -5671,10 +5683,10 @@
         <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -5718,7 +5730,7 @@
         <v>400</v>
       </c>
       <c r="Q36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -5729,10 +5741,10 @@
         <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>89</v>
@@ -5783,10 +5795,10 @@
         <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
@@ -5838,10 +5850,10 @@
         <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F39" t="s">
         <v>111</v>
@@ -5885,22 +5897,22 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40" t="s">
         <v>127</v>
-      </c>
-      <c r="B40" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" t="s">
-        <v>165</v>
-      </c>
-      <c r="D40" t="s">
-        <v>158</v>
-      </c>
-      <c r="E40" t="s">
-        <v>130</v>
-      </c>
-      <c r="F40" t="s">
-        <v>129</v>
       </c>
       <c r="G40" t="s">
         <v>15</v>
@@ -5936,30 +5948,30 @@
         <v>100</v>
       </c>
       <c r="Q40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E41" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G41" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H41">
         <f>$E$4+$E$5</f>
@@ -5993,30 +6005,30 @@
         <v>100</v>
       </c>
       <c r="Q41" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
       <c r="C42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H42">
         <f>$E$4+$E$5</f>
@@ -6050,27 +6062,27 @@
         <v>100</v>
       </c>
       <c r="Q42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G43" t="s">
         <v>67</v>
@@ -6107,7 +6119,67 @@
         <v>50</v>
       </c>
       <c r="Q43" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" t="s">
+        <v>143</v>
+      </c>
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44">
+        <v>2024</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>0.25</v>
+      </c>
+      <c r="L44">
+        <f t="shared" ref="L44" si="23">ROUNDDOWN(H44+I44+J44*(1-K44),0)</f>
+        <v>2026</v>
+      </c>
+      <c r="M44">
+        <f t="shared" ref="M44" si="24">L44-H44</f>
+        <v>2</v>
+      </c>
+      <c r="N44">
+        <v>25</v>
+      </c>
+      <c r="O44">
+        <v>2000</v>
+      </c>
+      <c r="P44">
+        <v>25</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -6125,7 +6197,7 @@
     </row>
     <row r="49" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I49" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J49">
         <v>4</v>
@@ -6189,7 +6261,7 @@
     </row>
     <row r="57" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I57" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J57">
         <v>1</v>
@@ -6213,7 +6285,7 @@
     </row>
     <row r="60" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I60" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J60">
         <v>2</v>
@@ -6253,7 +6325,7 @@
     </row>
     <row r="65" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I65" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J65">
         <v>1</v>
@@ -6261,7 +6333,7 @@
     </row>
     <row r="66" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I66" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J66">
         <v>2</v>

</xml_diff>

<commit_message>
Reverted flange facility back to Scenario
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_max.xlsx
+++ b/fabrication_ports/ports_scenario_max.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C5C579-0F48-465F-A076-93C3C06BEAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E4D4EC-3D89-482E-8B92-B3DB69782569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3696,7 +3696,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="I48:J67" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -4112,8 +4112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5903,7 +5903,7 @@
         <v>126</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D40" t="s">
         <v>156</v>

</xml_diff>

<commit_message>
Update port/vessel investments per peer review
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_max.xlsx
+++ b/fabrication_ports/ports_scenario_max.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E4D4EC-3D89-482E-8B92-B3DB69782569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CAA542-FB82-4B4F-AF0C-45B7D579D91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="1" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3696,7 +3696,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="I48:J67" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -4112,8 +4112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6116,7 +6116,7 @@
         <v>2000</v>
       </c>
       <c r="P43">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="Q43" t="s">
         <v>132</v>
@@ -6171,7 +6171,7 @@
         <v>2000</v>
       </c>
       <c r="P44">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="Q44" t="s">
         <v>171</v>

</xml_diff>